<commit_message>
add test case GetListRaiinInf
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/AccountingRepository/AccountingRepositorySample.xlsx
+++ b/CloudTest/SampleData/AccountingRepository/AccountingRepositorySample.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmartKarteBE\emr-cloud-be\CloudTest\SampleData\AccountingRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8E87C6-1B7A-45D8-B29B-D2561E6F6071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE1CBA1-5C6F-49A8-B68C-D2F259A2784A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{307AD4EF-97D7-4800-B587-784226BD97E2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{307AD4EF-97D7-4800-B587-784226BD97E2}"/>
   </bookViews>
   <sheets>
     <sheet name="RaiinInf" sheetId="1" r:id="rId1"/>
+    <sheet name="KaikeiInf" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="77">
   <si>
     <t>hp_id</t>
   </si>
@@ -133,6 +134,129 @@
   </si>
   <si>
     <t>2018-08-07 00:00:00.000 +0700</t>
+  </si>
+  <si>
+    <t>tensu</t>
+  </si>
+  <si>
+    <t>total_iryohi</t>
+  </si>
+  <si>
+    <t>pt_futan</t>
+  </si>
+  <si>
+    <t>jihi_futan</t>
+  </si>
+  <si>
+    <t>jihi_tax</t>
+  </si>
+  <si>
+    <t>jihi_outtax</t>
+  </si>
+  <si>
+    <t>adjust_futan</t>
+  </si>
+  <si>
+    <t>adjust_round</t>
+  </si>
+  <si>
+    <t>total_pt_futan</t>
+  </si>
+  <si>
+    <t>adjust_futan_val</t>
+  </si>
+  <si>
+    <t>adjust_futan_range</t>
+  </si>
+  <si>
+    <t>adjust_rate_val</t>
+  </si>
+  <si>
+    <t>adjust_rate_range</t>
+  </si>
+  <si>
+    <t>hoken_id</t>
+  </si>
+  <si>
+    <t>kohi1_id</t>
+  </si>
+  <si>
+    <t>kohi2_id</t>
+  </si>
+  <si>
+    <t>kohi3_id</t>
+  </si>
+  <si>
+    <t>kohi4_id</t>
+  </si>
+  <si>
+    <t>hoken_kbn</t>
+  </si>
+  <si>
+    <t>hoken_sbt_cd</t>
+  </si>
+  <si>
+    <t>rece_sbt</t>
+  </si>
+  <si>
+    <t>houbetu</t>
+  </si>
+  <si>
+    <t>kohi1_houbetu</t>
+  </si>
+  <si>
+    <t>kohi2_houbetu</t>
+  </si>
+  <si>
+    <t>kohi3_houbetu</t>
+  </si>
+  <si>
+    <t>kohi4_houbetu</t>
+  </si>
+  <si>
+    <t>honke_kbn</t>
+  </si>
+  <si>
+    <t>jihi_futan_taxfree</t>
+  </si>
+  <si>
+    <t>jihi_futan_tax_nr</t>
+  </si>
+  <si>
+    <t>jihi_futan_tax_gen</t>
+  </si>
+  <si>
+    <t>jihi_futan_outtax_nr</t>
+  </si>
+  <si>
+    <t>jihi_futan_outtax_gen</t>
+  </si>
+  <si>
+    <t>jihi_tax_nr</t>
+  </si>
+  <si>
+    <t>jihi_tax_gen</t>
+  </si>
+  <si>
+    <t>jihi_outtax_nr</t>
+  </si>
+  <si>
+    <t>jihi_outtax_gen</t>
+  </si>
+  <si>
+    <t>hoken_rate</t>
+  </si>
+  <si>
+    <t>pt_rate</t>
+  </si>
+  <si>
+    <t>disp_rate</t>
+  </si>
+  <si>
+    <t>285YMMTSVR</t>
+  </si>
+  <si>
+    <t>13x8</t>
   </si>
 </sst>
 </file>
@@ -168,8 +292,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6BD0EE-0FF7-40B9-AEBC-E7F39445C802}">
   <dimension ref="A1:AI3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -790,4 +915,294 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F9D4AE-E736-45E9-8426-8EE35E0331BD}">
+  <dimension ref="A1:AT2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1" t="s">
+        <v>46</v>
+      </c>
+      <c r="S1" t="s">
+        <v>47</v>
+      </c>
+      <c r="T1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U1" t="s">
+        <v>49</v>
+      </c>
+      <c r="V1" t="s">
+        <v>50</v>
+      </c>
+      <c r="W1" t="s">
+        <v>51</v>
+      </c>
+      <c r="X1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>998</v>
+      </c>
+      <c r="B2">
+        <v>12345</v>
+      </c>
+      <c r="C2">
+        <v>20180807</v>
+      </c>
+      <c r="D2">
+        <v>1234321</v>
+      </c>
+      <c r="E2">
+        <v>2055</v>
+      </c>
+      <c r="F2">
+        <v>20550</v>
+      </c>
+      <c r="G2">
+        <v>500</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>500</v>
+      </c>
+      <c r="N2" s="1">
+        <v>44451.58668497685</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>100</v>
+      </c>
+      <c r="V2">
+        <v>101</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>2</v>
+      </c>
+      <c r="AA2">
+        <v>322</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC2">
+        <v>39</v>
+      </c>
+      <c r="AD2">
+        <v>80</v>
+      </c>
+      <c r="AH2">
+        <v>1</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AR2">
+        <v>10</v>
+      </c>
+      <c r="AS2">
+        <v>10</v>
+      </c>
+      <c r="AT2">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add test case FindPtHokenPatternList
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/AccountingRepository/AccountingRepositorySample.xlsx
+++ b/CloudTest/SampleData/AccountingRepository/AccountingRepositorySample.xlsx
@@ -8,13 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmartKarteBE\emr-cloud-be\CloudTest\SampleData\AccountingRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE1CBA1-5C6F-49A8-B68C-D2F259A2784A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC26D69B-AC74-489C-B77B-863640BA2763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{307AD4EF-97D7-4800-B587-784226BD97E2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="7" xr2:uid="{307AD4EF-97D7-4800-B587-784226BD97E2}"/>
   </bookViews>
   <sheets>
     <sheet name="RaiinInf" sheetId="1" r:id="rId1"/>
     <sheet name="KaikeiInf" sheetId="2" r:id="rId2"/>
+    <sheet name="PtInf" sheetId="3" r:id="rId3"/>
+    <sheet name="PtHokenInf" sheetId="4" r:id="rId4"/>
+    <sheet name="PtKohi" sheetId="6" r:id="rId5"/>
+    <sheet name="HokenMst" sheetId="8" r:id="rId6"/>
+    <sheet name="PtHokenPattern" sheetId="5" r:id="rId7"/>
+    <sheet name="PtHokenCheck" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="225">
   <si>
     <t>hp_id</t>
   </si>
@@ -257,6 +263,450 @@
   </si>
   <si>
     <t>13x8</t>
+  </si>
+  <si>
+    <t>seq_no</t>
+  </si>
+  <si>
+    <t>pt_num</t>
+  </si>
+  <si>
+    <t>kana_name</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>birthday</t>
+  </si>
+  <si>
+    <t>is_dead</t>
+  </si>
+  <si>
+    <t>death_date</t>
+  </si>
+  <si>
+    <t>home_post</t>
+  </si>
+  <si>
+    <t>home_address1</t>
+  </si>
+  <si>
+    <t>home_address2</t>
+  </si>
+  <si>
+    <t>tel1</t>
+  </si>
+  <si>
+    <t>tel2</t>
+  </si>
+  <si>
+    <t>mail</t>
+  </si>
+  <si>
+    <t>setainusi</t>
+  </si>
+  <si>
+    <t>zokugara</t>
+  </si>
+  <si>
+    <t>job</t>
+  </si>
+  <si>
+    <t>renraku_name</t>
+  </si>
+  <si>
+    <t>renraku_post</t>
+  </si>
+  <si>
+    <t>renraku_address1</t>
+  </si>
+  <si>
+    <t>renraku_address2</t>
+  </si>
+  <si>
+    <t>renraku_tel</t>
+  </si>
+  <si>
+    <t>renraku_memo</t>
+  </si>
+  <si>
+    <t>office_name</t>
+  </si>
+  <si>
+    <t>office_post</t>
+  </si>
+  <si>
+    <t>office_address1</t>
+  </si>
+  <si>
+    <t>office_address2</t>
+  </si>
+  <si>
+    <t>office_tel</t>
+  </si>
+  <si>
+    <t>office_memo</t>
+  </si>
+  <si>
+    <t>is_ryosyo_detail</t>
+  </si>
+  <si>
+    <t>primary_doctor</t>
+  </si>
+  <si>
+    <t>is_tester</t>
+  </si>
+  <si>
+    <t>is_delete</t>
+  </si>
+  <si>
+    <t>main_hoken_pid</t>
+  </si>
+  <si>
+    <t>reference_no</t>
+  </si>
+  <si>
+    <t>limit_cons_flg</t>
+  </si>
+  <si>
+    <t>quang anh</t>
+  </si>
+  <si>
+    <t>hoken_no</t>
+  </si>
+  <si>
+    <t>hoken_eda_no</t>
+  </si>
+  <si>
+    <t>hokensya_no</t>
+  </si>
+  <si>
+    <t>kigo</t>
+  </si>
+  <si>
+    <t>bango</t>
+  </si>
+  <si>
+    <t>hokensya_name</t>
+  </si>
+  <si>
+    <t>hokensya_post</t>
+  </si>
+  <si>
+    <t>hokensya_address</t>
+  </si>
+  <si>
+    <t>hokensya_tel</t>
+  </si>
+  <si>
+    <t>keizoku_kbn</t>
+  </si>
+  <si>
+    <t>sikaku_date</t>
+  </si>
+  <si>
+    <t>kofu_date</t>
+  </si>
+  <si>
+    <t>start_date</t>
+  </si>
+  <si>
+    <t>end_date</t>
+  </si>
+  <si>
+    <t>rate</t>
+  </si>
+  <si>
+    <t>gendogaku</t>
+  </si>
+  <si>
+    <t>kogaku_kbn</t>
+  </si>
+  <si>
+    <t>kogaku_type</t>
+  </si>
+  <si>
+    <t>tokurei_ym1</t>
+  </si>
+  <si>
+    <t>tokurei_ym2</t>
+  </si>
+  <si>
+    <t>tasukai_ym</t>
+  </si>
+  <si>
+    <t>syokumu_kbn</t>
+  </si>
+  <si>
+    <t>genmen_kbn</t>
+  </si>
+  <si>
+    <t>genmen_rate</t>
+  </si>
+  <si>
+    <t>genmen_gaku</t>
+  </si>
+  <si>
+    <t>tokki1</t>
+  </si>
+  <si>
+    <t>tokki2</t>
+  </si>
+  <si>
+    <t>tokki3</t>
+  </si>
+  <si>
+    <t>tokki4</t>
+  </si>
+  <si>
+    <t>tokki5</t>
+  </si>
+  <si>
+    <t>rousai_kofu_no</t>
+  </si>
+  <si>
+    <t>rousai_saigai_kbn</t>
+  </si>
+  <si>
+    <t>rousai_jigyosyo_name</t>
+  </si>
+  <si>
+    <t>rousai_pref_name</t>
+  </si>
+  <si>
+    <t>rousai_city_name</t>
+  </si>
+  <si>
+    <t>rousai_syobyo_date</t>
+  </si>
+  <si>
+    <t>rousai_syobyo_cd</t>
+  </si>
+  <si>
+    <t>rousai_roudou_cd</t>
+  </si>
+  <si>
+    <t>rousai_kantoku_cd</t>
+  </si>
+  <si>
+    <t>rousai_rece_count</t>
+  </si>
+  <si>
+    <t>jibai_hoken_name</t>
+  </si>
+  <si>
+    <t>jibai_hoken_tanto</t>
+  </si>
+  <si>
+    <t>jibai_hoken_tel</t>
+  </si>
+  <si>
+    <t>jibai_jyusyou_date</t>
+  </si>
+  <si>
+    <t>ryoyo_start_date</t>
+  </si>
+  <si>
+    <t>ryoyo_end_date</t>
+  </si>
+  <si>
+    <t>eda_no</t>
+  </si>
+  <si>
+    <t>é˜ªå›½æ±ä½</t>
+  </si>
+  <si>
+    <t>æ±ä½å‰åŒºï¼ˆå¤§é˜ªå¸‚ï¼‰</t>
+  </si>
+  <si>
+    <t>å¤§é˜ªå¸‚æ±ä½å‰åŒºæ±ç”°è¾ºï¼‘ï¼ï¼‘ï¼“ï¼ï¼”</t>
+  </si>
+  <si>
+    <t>06-4399-9625</t>
+  </si>
+  <si>
+    <t>hoken_memo</t>
+  </si>
+  <si>
+    <t>pref_no</t>
+  </si>
+  <si>
+    <t>futansya_no</t>
+  </si>
+  <si>
+    <t>jyukyusya_no</t>
+  </si>
+  <si>
+    <t>tokusyu_no</t>
+  </si>
+  <si>
+    <t>hoken_sbt_kbn</t>
+  </si>
+  <si>
+    <t>hoken_grp</t>
+  </si>
+  <si>
+    <t>check_date</t>
+  </si>
+  <si>
+    <t>check_id</t>
+  </si>
+  <si>
+    <t>check_machine</t>
+  </si>
+  <si>
+    <t>check_cmt</t>
+  </si>
+  <si>
+    <t>Check Comment</t>
+  </si>
+  <si>
+    <t>sort_no</t>
+  </si>
+  <si>
+    <t>hoken_name</t>
+  </si>
+  <si>
+    <t>hoken_sname</t>
+  </si>
+  <si>
+    <t>hoken_name_cd</t>
+  </si>
+  <si>
+    <t>check_digit</t>
+  </si>
+  <si>
+    <t>jyukyu_check_digit</t>
+  </si>
+  <si>
+    <t>is_futansya_no_check</t>
+  </si>
+  <si>
+    <t>is_jyukyusya_no_check</t>
+  </si>
+  <si>
+    <t>is_tokusyu_no_check</t>
+  </si>
+  <si>
+    <t>is_limit_list</t>
+  </si>
+  <si>
+    <t>is_limit_list_sum</t>
+  </si>
+  <si>
+    <t>is_other_pref_valid</t>
+  </si>
+  <si>
+    <t>age_start</t>
+  </si>
+  <si>
+    <t>age_end</t>
+  </si>
+  <si>
+    <t>en_ten</t>
+  </si>
+  <si>
+    <t>seikyu_ym</t>
+  </si>
+  <si>
+    <t>rece_sp_kbn</t>
+  </si>
+  <si>
+    <t>rece_seikyu_kbn</t>
+  </si>
+  <si>
+    <t>rece_futan_round</t>
+  </si>
+  <si>
+    <t>rece_kisai</t>
+  </si>
+  <si>
+    <t>rece_zero_kisai</t>
+  </si>
+  <si>
+    <t>rece_futan_kbn</t>
+  </si>
+  <si>
+    <t>rece_ten_kisai</t>
+  </si>
+  <si>
+    <t>calc_sp_kbn</t>
+  </si>
+  <si>
+    <t>limit_kbn</t>
+  </si>
+  <si>
+    <t>count_kbn</t>
+  </si>
+  <si>
+    <t>futan_kbn</t>
+  </si>
+  <si>
+    <t>futan_rate</t>
+  </si>
+  <si>
+    <t>kai_futangaku</t>
+  </si>
+  <si>
+    <t>kai_limit_futan</t>
+  </si>
+  <si>
+    <t>day_limit_futan</t>
+  </si>
+  <si>
+    <t>day_limit_count</t>
+  </si>
+  <si>
+    <t>month_limit_futan</t>
+  </si>
+  <si>
+    <t>month_limit_count</t>
+  </si>
+  <si>
+    <t>kogaku_tekiyo</t>
+  </si>
+  <si>
+    <t>hoken_kohi_kbn</t>
+  </si>
+  <si>
+    <t>month_sp_limit</t>
+  </si>
+  <si>
+    <t>rece_kisai2</t>
+  </si>
+  <si>
+    <t>rece_futan_hide</t>
+  </si>
+  <si>
+    <t>kogaku_total_kbn</t>
+  </si>
+  <si>
+    <t>futan_yusen</t>
+  </si>
+  <si>
+    <t>kogaku_total_all</t>
+  </si>
+  <si>
+    <t>rece_kisai_kokho</t>
+  </si>
+  <si>
+    <t>kogaku_hairyo_kbn</t>
+  </si>
+  <si>
+    <t>kogaku_total_exc_futan</t>
+  </si>
+  <si>
+    <t>çœŒå°å…æ…¢æ€§</t>
+  </si>
+  <si>
+    <t>çœŒå°æ…¢0</t>
+  </si>
+  <si>
+    <t>çœŒå°æ…¢</t>
   </si>
 </sst>
 </file>
@@ -921,7 +1371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F9D4AE-E736-45E9-8426-8EE35E0331BD}">
   <dimension ref="A1:AT2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -1205,4 +1655,1331 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDBC675A-52CC-4FD5-9359-1C7B03C4FEC4}">
+  <dimension ref="A1:AR2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" t="s">
+        <v>86</v>
+      </c>
+      <c r="M1" t="s">
+        <v>87</v>
+      </c>
+      <c r="N1" t="s">
+        <v>88</v>
+      </c>
+      <c r="O1" t="s">
+        <v>89</v>
+      </c>
+      <c r="P1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>91</v>
+      </c>
+      <c r="R1" t="s">
+        <v>92</v>
+      </c>
+      <c r="S1" t="s">
+        <v>93</v>
+      </c>
+      <c r="T1" t="s">
+        <v>94</v>
+      </c>
+      <c r="U1" t="s">
+        <v>95</v>
+      </c>
+      <c r="V1" t="s">
+        <v>96</v>
+      </c>
+      <c r="W1" t="s">
+        <v>97</v>
+      </c>
+      <c r="X1" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>998</v>
+      </c>
+      <c r="B2">
+        <v>12345</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2222</v>
+      </c>
+      <c r="E2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>20020101</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>45034.017906608795</v>
+      </c>
+      <c r="AK2">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="1">
+        <v>45034.017906608795</v>
+      </c>
+      <c r="AN2">
+        <v>2</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
+      </c>
+      <c r="AQ2">
+        <v>712</v>
+      </c>
+      <c r="AR2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E4556A1-B621-4664-96E7-3F0E43EB4559}">
+  <dimension ref="A1:BI2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1" t="s">
+        <v>120</v>
+      </c>
+      <c r="O1" t="s">
+        <v>121</v>
+      </c>
+      <c r="P1" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>123</v>
+      </c>
+      <c r="R1" t="s">
+        <v>124</v>
+      </c>
+      <c r="S1" t="s">
+        <v>125</v>
+      </c>
+      <c r="T1" t="s">
+        <v>126</v>
+      </c>
+      <c r="U1" t="s">
+        <v>127</v>
+      </c>
+      <c r="V1" t="s">
+        <v>128</v>
+      </c>
+      <c r="W1" t="s">
+        <v>129</v>
+      </c>
+      <c r="X1" t="s">
+        <v>130</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>131</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>157</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>22</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>23</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>24</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>25</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>26</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>27</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>28</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>158</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>159</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>998</v>
+      </c>
+      <c r="B2">
+        <v>12345</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <v>60</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>274241</v>
+      </c>
+      <c r="H2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I2">
+        <v>547425</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>100</v>
+      </c>
+      <c r="M2" t="s">
+        <v>162</v>
+      </c>
+      <c r="N2">
+        <v>5468501</v>
+      </c>
+      <c r="O2" t="s">
+        <v>163</v>
+      </c>
+      <c r="P2" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>20190410</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AU2">
+        <v>0</v>
+      </c>
+      <c r="AY2">
+        <v>0</v>
+      </c>
+      <c r="AZ2">
+        <v>0</v>
+      </c>
+      <c r="BA2" s="1">
+        <v>40276.015474537038</v>
+      </c>
+      <c r="BB2">
+        <v>0</v>
+      </c>
+      <c r="BD2" s="1">
+        <v>44429.484398148146</v>
+      </c>
+      <c r="BE2">
+        <v>0</v>
+      </c>
+      <c r="BG2">
+        <v>0</v>
+      </c>
+      <c r="BH2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784E09D1-489B-460C-B1A3-268D47836302}">
+  <dimension ref="A1:Y2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="13.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" t="s">
+        <v>167</v>
+      </c>
+      <c r="I1" t="s">
+        <v>168</v>
+      </c>
+      <c r="J1" t="s">
+        <v>169</v>
+      </c>
+      <c r="K1" t="s">
+        <v>124</v>
+      </c>
+      <c r="L1" t="s">
+        <v>125</v>
+      </c>
+      <c r="M1" t="s">
+        <v>126</v>
+      </c>
+      <c r="N1" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1" t="s">
+        <v>128</v>
+      </c>
+      <c r="P1" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V1" t="s">
+        <v>27</v>
+      </c>
+      <c r="W1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" t="s">
+        <v>170</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>998</v>
+      </c>
+      <c r="B2">
+        <v>12345</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>27</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>41274242</v>
+      </c>
+      <c r="I2">
+        <v>1416841</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>99999999</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2" s="1">
+        <v>40276.015381944446</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="U2" s="1">
+        <v>40338.481620370374</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>7</v>
+      </c>
+      <c r="Y2">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73264705-026C-426F-AAEA-9DCC29056078}">
+  <dimension ref="A1:BG2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1" t="s">
+        <v>170</v>
+      </c>
+      <c r="I1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" t="s">
+        <v>178</v>
+      </c>
+      <c r="K1" t="s">
+        <v>179</v>
+      </c>
+      <c r="L1" t="s">
+        <v>180</v>
+      </c>
+      <c r="M1" t="s">
+        <v>181</v>
+      </c>
+      <c r="N1" t="s">
+        <v>182</v>
+      </c>
+      <c r="O1" t="s">
+        <v>183</v>
+      </c>
+      <c r="P1" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>185</v>
+      </c>
+      <c r="R1" t="s">
+        <v>186</v>
+      </c>
+      <c r="S1" t="s">
+        <v>187</v>
+      </c>
+      <c r="T1" t="s">
+        <v>188</v>
+      </c>
+      <c r="U1" t="s">
+        <v>189</v>
+      </c>
+      <c r="V1" t="s">
+        <v>190</v>
+      </c>
+      <c r="W1" t="s">
+        <v>191</v>
+      </c>
+      <c r="X1" t="s">
+        <v>192</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>194</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>195</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>196</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>197</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>198</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>199</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>201</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>202</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>203</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>204</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>205</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>206</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>207</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>208</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>209</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>210</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>211</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>212</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>213</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>215</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>216</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>217</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>218</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>219</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>220</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>998</v>
+      </c>
+      <c r="B2">
+        <v>17</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>20150101</v>
+      </c>
+      <c r="F2">
+        <v>99999999</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <v>82</v>
+      </c>
+      <c r="J2" t="s">
+        <v>222</v>
+      </c>
+      <c r="K2" t="s">
+        <v>223</v>
+      </c>
+      <c r="L2" t="s">
+        <v>224</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>999</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>1</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>3</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
+      </c>
+      <c r="AQ2" s="1">
+        <v>42150</v>
+      </c>
+      <c r="AR2">
+        <v>99997</v>
+      </c>
+      <c r="AT2" s="1">
+        <v>42150</v>
+      </c>
+      <c r="AU2">
+        <v>99997</v>
+      </c>
+      <c r="AW2">
+        <v>11</v>
+      </c>
+      <c r="AX2">
+        <v>0</v>
+      </c>
+      <c r="AY2">
+        <v>0</v>
+      </c>
+      <c r="AZ2">
+        <v>1</v>
+      </c>
+      <c r="BA2">
+        <v>0</v>
+      </c>
+      <c r="BB2">
+        <v>0</v>
+      </c>
+      <c r="BC2">
+        <v>0</v>
+      </c>
+      <c r="BD2">
+        <v>0</v>
+      </c>
+      <c r="BE2">
+        <v>0</v>
+      </c>
+      <c r="BF2">
+        <v>0</v>
+      </c>
+      <c r="BG2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DCC4F9-9A0E-4512-87BF-391D2079D1C9}">
+  <dimension ref="A1:U2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" t="s">
+        <v>165</v>
+      </c>
+      <c r="M1" t="s">
+        <v>126</v>
+      </c>
+      <c r="N1" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>998</v>
+      </c>
+      <c r="B2">
+        <v>12345</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>211</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>20100414</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2" s="1">
+        <v>40276.015381944446</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1">
+        <v>40347.895416666666</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D9D0DAD-9F48-4AF4-816C-3E33CC5B4414}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H1" t="s">
+        <v>174</v>
+      </c>
+      <c r="I1" t="s">
+        <v>175</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>998</v>
+      </c>
+      <c r="B2">
+        <v>12345</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1">
+        <v>45373.291666666664</v>
+      </c>
+      <c r="G2">
+        <v>9999</v>
+      </c>
+      <c r="I2" t="s">
+        <v>176</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>45374.07494791667</v>
+      </c>
+      <c r="L2">
+        <v>9999</v>
+      </c>
+      <c r="N2" t="e">
+        <f>-infinity</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add test case GetListSyunoSeikyuTest
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/AccountingRepository/AccountingRepositorySample.xlsx
+++ b/CloudTest/SampleData/AccountingRepository/AccountingRepositorySample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmartKarteBE\emr-cloud-be\CloudTest\SampleData\AccountingRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC26D69B-AC74-489C-B77B-863640BA2763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D2C1C7-9FAA-4AC2-9020-CEB97F7FE435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="7" xr2:uid="{307AD4EF-97D7-4800-B587-784226BD97E2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="2" activeTab="9" xr2:uid="{307AD4EF-97D7-4800-B587-784226BD97E2}"/>
   </bookViews>
   <sheets>
     <sheet name="RaiinInf" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,8 @@
     <sheet name="HokenMst" sheetId="8" r:id="rId6"/>
     <sheet name="PtHokenPattern" sheetId="5" r:id="rId7"/>
     <sheet name="PtHokenCheck" sheetId="7" r:id="rId8"/>
+    <sheet name="SyunoSeikyu" sheetId="9" r:id="rId9"/>
+    <sheet name="SyunoNyukin" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="240">
   <si>
     <t>hp_id</t>
   </si>
@@ -707,6 +709,51 @@
   </si>
   <si>
     <t>çœŒå°æ…¢</t>
+  </si>
+  <si>
+    <t>nyukin_kbn</t>
+  </si>
+  <si>
+    <t>seikyu_tensu</t>
+  </si>
+  <si>
+    <t>seikyu_gaku</t>
+  </si>
+  <si>
+    <t>seikyu_detail</t>
+  </si>
+  <si>
+    <t>new_seikyu_tensu</t>
+  </si>
+  <si>
+    <t>new_seikyu_gaku</t>
+  </si>
+  <si>
+    <t>new_seikyu_detail</t>
+  </si>
+  <si>
+    <t>new_adjust_futan</t>
+  </si>
+  <si>
+    <t>nyukin_gaku</t>
+  </si>
+  <si>
+    <t>payment_method_cd</t>
+  </si>
+  <si>
+    <t>nyukin_cmt</t>
+  </si>
+  <si>
+    <t>nyukin_date</t>
+  </si>
+  <si>
+    <t>nyukinji_tensu</t>
+  </si>
+  <si>
+    <t>nyukinji_seikyu</t>
+  </si>
+  <si>
+    <t>nyukinji_detail</t>
   </si>
 </sst>
 </file>
@@ -1367,12 +1414,151 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66D63322-5432-4757-B737-25FB98527A39}">
+  <dimension ref="A1:V2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
+        <v>233</v>
+      </c>
+      <c r="H1" t="s">
+        <v>234</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>235</v>
+      </c>
+      <c r="K1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" t="s">
+        <v>77</v>
+      </c>
+      <c r="S1" t="s">
+        <v>236</v>
+      </c>
+      <c r="T1" t="s">
+        <v>237</v>
+      </c>
+      <c r="U1" t="s">
+        <v>238</v>
+      </c>
+      <c r="V1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>998</v>
+      </c>
+      <c r="B2">
+        <v>1234321</v>
+      </c>
+      <c r="C2">
+        <v>12345</v>
+      </c>
+      <c r="D2">
+        <v>20180807</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>40330</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1">
+        <v>40330</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>20100601</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F9D4AE-E736-45E9-8426-8EE35E0331BD}">
   <dimension ref="A1:AT2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2878,7 +3064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D9D0DAD-9F48-4AF4-816C-3E33CC5B4414}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
@@ -2982,4 +3168,130 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0855B1ED-BC61-48F0-AF1D-D7FB68813CD2}">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F1" t="s">
+        <v>226</v>
+      </c>
+      <c r="G1" t="s">
+        <v>227</v>
+      </c>
+      <c r="H1" t="s">
+        <v>228</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>229</v>
+      </c>
+      <c r="P1" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>231</v>
+      </c>
+      <c r="R1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>998</v>
+      </c>
+      <c r="B2">
+        <v>12345</v>
+      </c>
+      <c r="C2">
+        <v>20180807</v>
+      </c>
+      <c r="D2">
+        <v>1234321</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1144</v>
+      </c>
+      <c r="G2">
+        <v>3430</v>
+      </c>
+      <c r="I2" s="1">
+        <v>40413</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>40428</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>1144</v>
+      </c>
+      <c r="P2">
+        <v>3430</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add test case GetListKohiByKohiId
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/AccountingRepository/AccountingRepositorySample.xlsx
+++ b/CloudTest/SampleData/AccountingRepository/AccountingRepositorySample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmartKarteBE\emr-cloud-be\CloudTest\SampleData\AccountingRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D2C1C7-9FAA-4AC2-9020-CEB97F7FE435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECF51F2-9DF7-4F6B-901D-888D7F0B3D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="2" activeTab="9" xr2:uid="{307AD4EF-97D7-4800-B587-784226BD97E2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="2" activeTab="5" xr2:uid="{307AD4EF-97D7-4800-B587-784226BD97E2}"/>
   </bookViews>
   <sheets>
     <sheet name="RaiinInf" sheetId="1" r:id="rId1"/>
@@ -18,11 +18,12 @@
     <sheet name="PtInf" sheetId="3" r:id="rId3"/>
     <sheet name="PtHokenInf" sheetId="4" r:id="rId4"/>
     <sheet name="PtKohi" sheetId="6" r:id="rId5"/>
-    <sheet name="HokenMst" sheetId="8" r:id="rId6"/>
-    <sheet name="PtHokenPattern" sheetId="5" r:id="rId7"/>
-    <sheet name="PtHokenCheck" sheetId="7" r:id="rId8"/>
-    <sheet name="SyunoSeikyu" sheetId="9" r:id="rId9"/>
-    <sheet name="SyunoNyukin" sheetId="10" r:id="rId10"/>
+    <sheet name="HpInf" sheetId="11" r:id="rId6"/>
+    <sheet name="HokenMst" sheetId="8" r:id="rId7"/>
+    <sheet name="PtHokenPattern" sheetId="5" r:id="rId8"/>
+    <sheet name="PtHokenCheck" sheetId="7" r:id="rId9"/>
+    <sheet name="SyunoSeikyu" sheetId="9" r:id="rId10"/>
+    <sheet name="SyunoNyukin" sheetId="10" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="257">
   <si>
     <t>hp_id</t>
   </si>
@@ -754,6 +755,57 @@
   </si>
   <si>
     <t>nyukinji_detail</t>
+  </si>
+  <si>
+    <t>hp_cd</t>
+  </si>
+  <si>
+    <t>rousai_hp_cd</t>
+  </si>
+  <si>
+    <t>hp_name</t>
+  </si>
+  <si>
+    <t>rece_hp_name</t>
+  </si>
+  <si>
+    <t>kaisetu_name</t>
+  </si>
+  <si>
+    <t>post_cd</t>
+  </si>
+  <si>
+    <t>address1</t>
+  </si>
+  <si>
+    <t>address2</t>
+  </si>
+  <si>
+    <t>tel</t>
+  </si>
+  <si>
+    <t>fax_no</t>
+  </si>
+  <si>
+    <t>other_contacts</t>
+  </si>
+  <si>
+    <t>sfdffsj</t>
+  </si>
+  <si>
+    <t>sfdffsjfklsjrpoiqewrejksdfjalkjfdjfqwoiejfljlskdjfldsjflsdjfljfoiwjeoijoiewjiore</t>
+  </si>
+  <si>
+    <t>sfdffsjfklsjrpoiqewrejksdfjalkjfdjfqwoie</t>
+  </si>
+  <si>
+    <t>sfdffsjfklsjrpoiqewrejksdfjalkjfdjfqwoiejfljlskdjfldsjflsdjfljfoiwjeoijoiewjiorewjroiewjroiewjroiewj</t>
+  </si>
+  <si>
+    <t>sfdffsjfklsjrpo</t>
+  </si>
+  <si>
+    <t>abcd</t>
   </si>
 </sst>
 </file>
@@ -1415,10 +1467,136 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0855B1ED-BC61-48F0-AF1D-D7FB68813CD2}">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F1" t="s">
+        <v>226</v>
+      </c>
+      <c r="G1" t="s">
+        <v>227</v>
+      </c>
+      <c r="H1" t="s">
+        <v>228</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>229</v>
+      </c>
+      <c r="P1" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>231</v>
+      </c>
+      <c r="R1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>998</v>
+      </c>
+      <c r="B2">
+        <v>12345</v>
+      </c>
+      <c r="C2">
+        <v>20180807</v>
+      </c>
+      <c r="D2">
+        <v>1234321</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1144</v>
+      </c>
+      <c r="G2">
+        <v>3430</v>
+      </c>
+      <c r="I2" s="1">
+        <v>40413</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>40428</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>1144</v>
+      </c>
+      <c r="P2">
+        <v>3430</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66D63322-5432-4757-B737-25FB98527A39}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -2552,11 +2730,138 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26DFBEB-5F16-4505-AAA1-07062F422922}">
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E1" t="s">
+        <v>242</v>
+      </c>
+      <c r="F1" t="s">
+        <v>243</v>
+      </c>
+      <c r="G1" t="s">
+        <v>244</v>
+      </c>
+      <c r="H1" t="s">
+        <v>245</v>
+      </c>
+      <c r="I1" t="s">
+        <v>166</v>
+      </c>
+      <c r="J1" t="s">
+        <v>246</v>
+      </c>
+      <c r="K1" t="s">
+        <v>247</v>
+      </c>
+      <c r="L1" t="s">
+        <v>248</v>
+      </c>
+      <c r="M1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S1" t="s">
+        <v>249</v>
+      </c>
+      <c r="T1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>998</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E2" t="s">
+        <v>252</v>
+      </c>
+      <c r="F2" t="s">
+        <v>252</v>
+      </c>
+      <c r="G2" t="s">
+        <v>253</v>
+      </c>
+      <c r="H2">
+        <v>1231232</v>
+      </c>
+      <c r="I2">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>254</v>
+      </c>
+      <c r="K2" t="s">
+        <v>254</v>
+      </c>
+      <c r="L2" t="s">
+        <v>255</v>
+      </c>
+      <c r="M2" s="1">
+        <v>45040.84794363426</v>
+      </c>
+      <c r="N2">
+        <v>2</v>
+      </c>
+      <c r="P2" s="1">
+        <v>45184.049576296296</v>
+      </c>
+      <c r="Q2">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73264705-026C-426F-AAEA-9DCC29056078}">
   <dimension ref="A1:BG2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2921,7 +3226,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DCC4F9-9A0E-4512-87BF-391D2079D1C9}">
   <dimension ref="A1:U2"/>
   <sheetViews>
@@ -3060,7 +3365,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D9D0DAD-9F48-4AF4-816C-3E33CC5B4414}">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -3168,130 +3473,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0855B1ED-BC61-48F0-AF1D-D7FB68813CD2}">
-  <dimension ref="A1:S2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>225</v>
-      </c>
-      <c r="F1" t="s">
-        <v>226</v>
-      </c>
-      <c r="G1" t="s">
-        <v>227</v>
-      </c>
-      <c r="H1" t="s">
-        <v>228</v>
-      </c>
-      <c r="I1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" t="s">
-        <v>229</v>
-      </c>
-      <c r="P1" t="s">
-        <v>230</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>231</v>
-      </c>
-      <c r="R1" t="s">
-        <v>42</v>
-      </c>
-      <c r="S1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>998</v>
-      </c>
-      <c r="B2">
-        <v>12345</v>
-      </c>
-      <c r="C2">
-        <v>20180807</v>
-      </c>
-      <c r="D2">
-        <v>1234321</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1144</v>
-      </c>
-      <c r="G2">
-        <v>3430</v>
-      </c>
-      <c r="I2" s="1">
-        <v>40413</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="L2" s="1">
-        <v>40428</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>1144</v>
-      </c>
-      <c r="P2">
-        <v>3430</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add test case GetAccountingInf, GetVisibilityPtKohiModelList
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/AccountingRepository/AccountingRepositorySample.xlsx
+++ b/CloudTest/SampleData/AccountingRepository/AccountingRepositorySample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmartKarteBE\emr-cloud-be\CloudTest\SampleData\AccountingRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECF51F2-9DF7-4F6B-901D-888D7F0B3D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49089B0-487E-4611-A30F-62626D2A9B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="2" activeTab="5" xr2:uid="{307AD4EF-97D7-4800-B587-784226BD97E2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{307AD4EF-97D7-4800-B587-784226BD97E2}"/>
   </bookViews>
   <sheets>
     <sheet name="RaiinInf" sheetId="1" r:id="rId1"/>
@@ -1160,8 +1160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6BD0EE-0FF7-40B9-AEBC-E7F39445C802}">
   <dimension ref="A1:AI3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1735,8 +1735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F9D4AE-E736-45E9-8426-8EE35E0331BD}">
   <dimension ref="A1:AT2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1950,16 +1950,16 @@
         <v>100</v>
       </c>
       <c r="V2">
-        <v>101</v>
+        <v>10</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="X2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="Y2">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="Z2">
         <v>2</v>
@@ -2733,7 +2733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26DFBEB-5F16-4505-AAA1-07062F422922}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
@@ -2861,12 +2861,13 @@
   <dimension ref="A1:BG2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="AN18" sqref="AN18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:59" x14ac:dyDescent="0.3">
@@ -3173,7 +3174,7 @@
         <v>0</v>
       </c>
       <c r="AP2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ2" s="1">
         <v>42150</v>

</xml_diff>

<commit_message>
add test case Validate SaveAccounting
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/AccountingRepository/AccountingRepositorySample.xlsx
+++ b/CloudTest/SampleData/AccountingRepository/AccountingRepositorySample.xlsx
@@ -8,22 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmartKarteBE\emr-cloud-be\CloudTest\SampleData\AccountingRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49089B0-487E-4611-A30F-62626D2A9B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2651C5-3683-4889-8023-375B2ECB1C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{307AD4EF-97D7-4800-B587-784226BD97E2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{307AD4EF-97D7-4800-B587-784226BD97E2}"/>
   </bookViews>
   <sheets>
     <sheet name="RaiinInf" sheetId="1" r:id="rId1"/>
-    <sheet name="KaikeiInf" sheetId="2" r:id="rId2"/>
-    <sheet name="PtInf" sheetId="3" r:id="rId3"/>
-    <sheet name="PtHokenInf" sheetId="4" r:id="rId4"/>
-    <sheet name="PtKohi" sheetId="6" r:id="rId5"/>
-    <sheet name="HpInf" sheetId="11" r:id="rId6"/>
-    <sheet name="HokenMst" sheetId="8" r:id="rId7"/>
-    <sheet name="PtHokenPattern" sheetId="5" r:id="rId8"/>
-    <sheet name="PtHokenCheck" sheetId="7" r:id="rId9"/>
-    <sheet name="SyunoSeikyu" sheetId="9" r:id="rId10"/>
-    <sheet name="SyunoNyukin" sheetId="10" r:id="rId11"/>
+    <sheet name="UserMst" sheetId="12" r:id="rId2"/>
+    <sheet name="UserPermission" sheetId="13" r:id="rId3"/>
+    <sheet name="KaikeiInf" sheetId="2" r:id="rId4"/>
+    <sheet name="PtInf" sheetId="3" r:id="rId5"/>
+    <sheet name="PtHokenInf" sheetId="4" r:id="rId6"/>
+    <sheet name="PtKohi" sheetId="6" r:id="rId7"/>
+    <sheet name="HpInf" sheetId="11" r:id="rId8"/>
+    <sheet name="HokenMst" sheetId="8" r:id="rId9"/>
+    <sheet name="PtHokenPattern" sheetId="5" r:id="rId10"/>
+    <sheet name="PtHokenCheck" sheetId="7" r:id="rId11"/>
+    <sheet name="SyunoSeikyu" sheetId="9" r:id="rId12"/>
+    <sheet name="SyunoNyukin" sheetId="10" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="285">
   <si>
     <t>hp_id</t>
   </si>
@@ -806,6 +808,90 @@
   </si>
   <si>
     <t>abcd</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>job_cd</t>
+  </si>
+  <si>
+    <t>manager_kbn</t>
+  </si>
+  <si>
+    <t>sname</t>
+  </si>
+  <si>
+    <t>login_id</t>
+  </si>
+  <si>
+    <t>mayaku_license_no</t>
+  </si>
+  <si>
+    <t>renkei_cd1</t>
+  </si>
+  <si>
+    <t>dr_name</t>
+  </si>
+  <si>
+    <t>login_type</t>
+  </si>
+  <si>
+    <t>hpki_sn</t>
+  </si>
+  <si>
+    <t>hpki_issuer_dn</t>
+  </si>
+  <si>
+    <t>hash_password_byte</t>
+  </si>
+  <si>
+    <t>salt_byte</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>is_init_password</t>
+  </si>
+  <si>
+    <t>miss_login_count</t>
+  </si>
+  <si>
+    <t>hash_password</t>
+  </si>
+  <si>
+    <t>salt</t>
+  </si>
+  <si>
+    <t>ï½»ï½¸ï¾—ï½²Dr</t>
+  </si>
+  <si>
+    <t>æ«»äº•ã€€å…‹å®£</t>
+  </si>
+  <si>
+    <t>æ«»äº•Dr</t>
+  </si>
+  <si>
+    <t>ï¿½ï¿½_x0001_?ï¿½ï¿½ï¿½ï¿½ï¿½ï¿½fï¿½Ç_x0003_ï¿½ï¿½3ï¿½ï¿½ï¿½ï¿½{ï¿½ï¿½ï¿½ï¿½wï¿½;_x0007_ï¿½</t>
+  </si>
+  <si>
+    <t>_x001E_ï¿½ï¿½_x0011_ï¿½ï¿½_x0008_ï¿½_x0005_ï¿½ï¿½*^1_x000B_ï¿½kï¿½BMï¿½ï¿½ï¿½ï¿½sZï¿½ÒŽ0{</t>
+  </si>
+  <si>
+    <t>B3C0013F84D1F7BEB0EF66A5C78103A9B5339D8B8EC37BAFDFFEA377F53B07E1</t>
+  </si>
+  <si>
+    <t>1EFEC90011998A08AE059FC32A5E310BD56BED424DF5CEFBFC735AEBD28E307B</t>
+  </si>
+  <si>
+    <t>function_cd</t>
+  </si>
+  <si>
+    <t>permission</t>
+  </si>
+  <si>
+    <t>03000000</t>
   </si>
 </sst>
 </file>
@@ -841,9 +927,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1160,7 +1247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6BD0EE-0FF7-40B9-AEBC-E7F39445C802}">
   <dimension ref="A1:AI3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -1467,6 +1554,255 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DCC4F9-9A0E-4512-87BF-391D2079D1C9}">
+  <dimension ref="A1:U2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" t="s">
+        <v>165</v>
+      </c>
+      <c r="M1" t="s">
+        <v>126</v>
+      </c>
+      <c r="N1" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>998</v>
+      </c>
+      <c r="B2">
+        <v>12345</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>211</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>20100414</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2" s="1">
+        <v>40276.015381944446</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1">
+        <v>40347.895416666666</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D9D0DAD-9F48-4AF4-816C-3E33CC5B4414}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H1" t="s">
+        <v>174</v>
+      </c>
+      <c r="I1" t="s">
+        <v>175</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>998</v>
+      </c>
+      <c r="B2">
+        <v>12345</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1">
+        <v>45373.291666666664</v>
+      </c>
+      <c r="G2">
+        <v>9999</v>
+      </c>
+      <c r="I2" t="s">
+        <v>176</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>45374.07494791667</v>
+      </c>
+      <c r="L2">
+        <v>9999</v>
+      </c>
+      <c r="N2" t="e">
+        <f>-infinity</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0855B1ED-BC61-48F0-AF1D-D7FB68813CD2}">
   <dimension ref="A1:S2"/>
   <sheetViews>
@@ -1592,7 +1928,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66D63322-5432-4757-B737-25FB98527A39}">
   <dimension ref="A1:V2"/>
   <sheetViews>
@@ -1732,6 +2068,282 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35AB2591-6C24-4001-94BB-19D57CBA9876}">
+  <dimension ref="A1:AG2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" t="s">
+        <v>260</v>
+      </c>
+      <c r="I1" t="s">
+        <v>261</v>
+      </c>
+      <c r="J1" t="s">
+        <v>262</v>
+      </c>
+      <c r="K1" t="s">
+        <v>126</v>
+      </c>
+      <c r="L1" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1" t="s">
+        <v>177</v>
+      </c>
+      <c r="N1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U1" t="s">
+        <v>263</v>
+      </c>
+      <c r="V1" t="s">
+        <v>264</v>
+      </c>
+      <c r="W1" t="s">
+        <v>265</v>
+      </c>
+      <c r="X1" t="s">
+        <v>266</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>267</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>268</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>269</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>270</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>271</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>272</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>273</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>998</v>
+      </c>
+      <c r="B2">
+        <v>96789049</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>275</v>
+      </c>
+      <c r="G2" t="s">
+        <v>276</v>
+      </c>
+      <c r="H2" t="s">
+        <v>277</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>99999999</v>
+      </c>
+      <c r="M2">
+        <v>12</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1">
+        <v>41362</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1">
+        <v>41362</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="V2" t="s">
+        <v>276</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>278</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>279</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>280</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE9B5002-AE00-4D99-91C6-53D26DE9CD9D}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="11.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="D1" t="s">
+        <v>283</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>998</v>
+      </c>
+      <c r="B2">
+        <v>96789049</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44450.834597685185</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>44450.834597685185</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F9D4AE-E736-45E9-8426-8EE35E0331BD}">
   <dimension ref="A1:AT2"/>
   <sheetViews>
@@ -2021,7 +2633,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDBC675A-52CC-4FD5-9359-1C7B03C4FEC4}">
   <dimension ref="A1:AR2"/>
   <sheetViews>
@@ -2235,7 +2847,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E4556A1-B621-4664-96E7-3F0E43EB4559}">
   <dimension ref="A1:BI2"/>
   <sheetViews>
@@ -2566,7 +3178,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784E09D1-489B-460C-B1A3-268D47836302}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
@@ -2729,7 +3341,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26DFBEB-5F16-4505-AAA1-07062F422922}">
   <dimension ref="A1:T2"/>
   <sheetViews>
@@ -2856,7 +3468,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73264705-026C-426F-AAEA-9DCC29056078}">
   <dimension ref="A1:BG2"/>
   <sheetViews>
@@ -3225,253 +3837,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DCC4F9-9A0E-4512-87BF-391D2079D1C9}">
-  <dimension ref="A1:U2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="10.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J1" t="s">
-        <v>52</v>
-      </c>
-      <c r="K1" t="s">
-        <v>53</v>
-      </c>
-      <c r="L1" t="s">
-        <v>165</v>
-      </c>
-      <c r="M1" t="s">
-        <v>126</v>
-      </c>
-      <c r="N1" t="s">
-        <v>127</v>
-      </c>
-      <c r="O1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>24</v>
-      </c>
-      <c r="R1" t="s">
-        <v>25</v>
-      </c>
-      <c r="S1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>998</v>
-      </c>
-      <c r="B2">
-        <v>12345</v>
-      </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>9</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>211</v>
-      </c>
-      <c r="G2">
-        <v>10</v>
-      </c>
-      <c r="H2">
-        <v>10</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>20100414</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2" s="1">
-        <v>40276.015381944446</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="S2" s="1">
-        <v>40347.895416666666</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D9D0DAD-9F48-4AF4-816C-3E33CC5B4414}">
-  <dimension ref="A1:P2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" t="s">
-        <v>172</v>
-      </c>
-      <c r="G1" t="s">
-        <v>173</v>
-      </c>
-      <c r="H1" t="s">
-        <v>174</v>
-      </c>
-      <c r="I1" t="s">
-        <v>175</v>
-      </c>
-      <c r="J1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>998</v>
-      </c>
-      <c r="B2">
-        <v>12345</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1">
-        <v>45373.291666666664</v>
-      </c>
-      <c r="G2">
-        <v>9999</v>
-      </c>
-      <c r="I2" t="s">
-        <v>176</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1">
-        <v>45374.07494791667</v>
-      </c>
-      <c r="L2">
-        <v>9999</v>
-      </c>
-      <c r="N2" t="e">
-        <f>-infinity</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add test case GetWarningMemoInteractor
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/AccountingRepository/AccountingRepositorySample.xlsx
+++ b/CloudTest/SampleData/AccountingRepository/AccountingRepositorySample.xlsx
@@ -8,24 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmartKarteBE\emr-cloud-be\CloudTest\SampleData\AccountingRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2651C5-3683-4889-8023-375B2ECB1C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7820192B-794B-4148-8D0B-58A26F7B50B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{307AD4EF-97D7-4800-B587-784226BD97E2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{307AD4EF-97D7-4800-B587-784226BD97E2}"/>
   </bookViews>
   <sheets>
     <sheet name="RaiinInf" sheetId="1" r:id="rId1"/>
     <sheet name="UserMst" sheetId="12" r:id="rId2"/>
     <sheet name="UserPermission" sheetId="13" r:id="rId3"/>
-    <sheet name="KaikeiInf" sheetId="2" r:id="rId4"/>
-    <sheet name="PtInf" sheetId="3" r:id="rId5"/>
-    <sheet name="PtHokenInf" sheetId="4" r:id="rId6"/>
-    <sheet name="PtKohi" sheetId="6" r:id="rId7"/>
-    <sheet name="HpInf" sheetId="11" r:id="rId8"/>
-    <sheet name="HokenMst" sheetId="8" r:id="rId9"/>
-    <sheet name="PtHokenPattern" sheetId="5" r:id="rId10"/>
-    <sheet name="PtHokenCheck" sheetId="7" r:id="rId11"/>
-    <sheet name="SyunoSeikyu" sheetId="9" r:id="rId12"/>
-    <sheet name="SyunoNyukin" sheetId="10" r:id="rId13"/>
+    <sheet name="CalcLog" sheetId="14" r:id="rId4"/>
+    <sheet name="KaikeiInf" sheetId="2" r:id="rId5"/>
+    <sheet name="PtInf" sheetId="3" r:id="rId6"/>
+    <sheet name="PtHokenInf" sheetId="4" r:id="rId7"/>
+    <sheet name="PtKohi" sheetId="6" r:id="rId8"/>
+    <sheet name="HpInf" sheetId="11" r:id="rId9"/>
+    <sheet name="HokenMst" sheetId="8" r:id="rId10"/>
+    <sheet name="PtHokenPattern" sheetId="5" r:id="rId11"/>
+    <sheet name="PtHokenCheck" sheetId="7" r:id="rId12"/>
+    <sheet name="SyunoSeikyu" sheetId="9" r:id="rId13"/>
+    <sheet name="SyunoNyukin" sheetId="10" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="295">
   <si>
     <t>hp_id</t>
   </si>
@@ -892,6 +893,36 @@
   </si>
   <si>
     <t>03000000</t>
+  </si>
+  <si>
+    <t>log_sbt</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>del_item_cd</t>
+  </si>
+  <si>
+    <t>del_sbt</t>
+  </si>
+  <si>
+    <t>is_warning</t>
+  </si>
+  <si>
+    <t>item_cd</t>
+  </si>
+  <si>
+    <t>term_cnt</t>
+  </si>
+  <si>
+    <t>term_sbt</t>
+  </si>
+  <si>
+    <t>SmartKarte</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -927,10 +958,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1554,6 +1586,377 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73264705-026C-426F-AAEA-9DCC29056078}">
+  <dimension ref="A1:BG2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AN18" sqref="AN18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="16.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1" t="s">
+        <v>170</v>
+      </c>
+      <c r="I1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" t="s">
+        <v>178</v>
+      </c>
+      <c r="K1" t="s">
+        <v>179</v>
+      </c>
+      <c r="L1" t="s">
+        <v>180</v>
+      </c>
+      <c r="M1" t="s">
+        <v>181</v>
+      </c>
+      <c r="N1" t="s">
+        <v>182</v>
+      </c>
+      <c r="O1" t="s">
+        <v>183</v>
+      </c>
+      <c r="P1" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>185</v>
+      </c>
+      <c r="R1" t="s">
+        <v>186</v>
+      </c>
+      <c r="S1" t="s">
+        <v>187</v>
+      </c>
+      <c r="T1" t="s">
+        <v>188</v>
+      </c>
+      <c r="U1" t="s">
+        <v>189</v>
+      </c>
+      <c r="V1" t="s">
+        <v>190</v>
+      </c>
+      <c r="W1" t="s">
+        <v>191</v>
+      </c>
+      <c r="X1" t="s">
+        <v>192</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>194</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>195</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>196</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>197</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>198</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>199</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>201</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>202</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>203</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>204</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>205</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>206</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>207</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>208</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>209</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>210</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>211</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>212</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>213</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>215</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>216</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>217</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>218</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>219</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>220</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>998</v>
+      </c>
+      <c r="B2">
+        <v>17</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>20150101</v>
+      </c>
+      <c r="F2">
+        <v>99999999</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <v>82</v>
+      </c>
+      <c r="J2" t="s">
+        <v>222</v>
+      </c>
+      <c r="K2" t="s">
+        <v>223</v>
+      </c>
+      <c r="L2" t="s">
+        <v>224</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>999</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>1</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>3</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <v>1</v>
+      </c>
+      <c r="AQ2" s="1">
+        <v>42150</v>
+      </c>
+      <c r="AR2">
+        <v>99997</v>
+      </c>
+      <c r="AT2" s="1">
+        <v>42150</v>
+      </c>
+      <c r="AU2">
+        <v>99997</v>
+      </c>
+      <c r="AW2">
+        <v>11</v>
+      </c>
+      <c r="AX2">
+        <v>0</v>
+      </c>
+      <c r="AY2">
+        <v>0</v>
+      </c>
+      <c r="AZ2">
+        <v>1</v>
+      </c>
+      <c r="BA2">
+        <v>0</v>
+      </c>
+      <c r="BB2">
+        <v>0</v>
+      </c>
+      <c r="BC2">
+        <v>0</v>
+      </c>
+      <c r="BD2">
+        <v>0</v>
+      </c>
+      <c r="BE2">
+        <v>0</v>
+      </c>
+      <c r="BF2">
+        <v>0</v>
+      </c>
+      <c r="BG2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DCC4F9-9A0E-4512-87BF-391D2079D1C9}">
   <dimension ref="A1:U2"/>
   <sheetViews>
@@ -1692,7 +2095,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D9D0DAD-9F48-4AF4-816C-3E33CC5B4414}">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -1802,7 +2205,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0855B1ED-BC61-48F0-AF1D-D7FB68813CD2}">
   <dimension ref="A1:S2"/>
   <sheetViews>
@@ -1928,7 +2331,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66D63322-5432-4757-B737-25FB98527A39}">
   <dimension ref="A1:V2"/>
   <sheetViews>
@@ -2270,7 +2673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE9B5002-AE00-4D99-91C6-53D26DE9CD9D}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -2344,6 +2747,142 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33A48F04-CF42-4200-84BC-DF9962C3CD4A}">
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G1" t="s">
+        <v>286</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" t="s">
+        <v>287</v>
+      </c>
+      <c r="O1" t="s">
+        <v>288</v>
+      </c>
+      <c r="P1" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R1" t="s">
+        <v>290</v>
+      </c>
+      <c r="S1" t="s">
+        <v>291</v>
+      </c>
+      <c r="T1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>998</v>
+      </c>
+      <c r="B2">
+        <v>12345</v>
+      </c>
+      <c r="C2">
+        <v>1234321</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>20180807</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="H2" s="1">
+        <v>45044.845445567131</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>293</v>
+      </c>
+      <c r="K2" s="1">
+        <v>45044.845445567131</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+      <c r="M2" t="s">
+        <v>293</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F9D4AE-E736-45E9-8426-8EE35E0331BD}">
   <dimension ref="A1:AT2"/>
   <sheetViews>
@@ -2633,7 +3172,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDBC675A-52CC-4FD5-9359-1C7B03C4FEC4}">
   <dimension ref="A1:AR2"/>
   <sheetViews>
@@ -2847,7 +3386,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E4556A1-B621-4664-96E7-3F0E43EB4559}">
   <dimension ref="A1:BI2"/>
   <sheetViews>
@@ -3178,7 +3717,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784E09D1-489B-460C-B1A3-268D47836302}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
@@ -3341,7 +3880,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26DFBEB-5F16-4505-AAA1-07062F422922}">
   <dimension ref="A1:T2"/>
   <sheetViews>
@@ -3466,375 +4005,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73264705-026C-426F-AAEA-9DCC29056078}">
-  <dimension ref="A1:BG2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AN18" sqref="AN18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="16.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F1" t="s">
-        <v>127</v>
-      </c>
-      <c r="G1" t="s">
-        <v>177</v>
-      </c>
-      <c r="H1" t="s">
-        <v>170</v>
-      </c>
-      <c r="I1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J1" t="s">
-        <v>178</v>
-      </c>
-      <c r="K1" t="s">
-        <v>179</v>
-      </c>
-      <c r="L1" t="s">
-        <v>180</v>
-      </c>
-      <c r="M1" t="s">
-        <v>181</v>
-      </c>
-      <c r="N1" t="s">
-        <v>182</v>
-      </c>
-      <c r="O1" t="s">
-        <v>183</v>
-      </c>
-      <c r="P1" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>185</v>
-      </c>
-      <c r="R1" t="s">
-        <v>186</v>
-      </c>
-      <c r="S1" t="s">
-        <v>187</v>
-      </c>
-      <c r="T1" t="s">
-        <v>188</v>
-      </c>
-      <c r="U1" t="s">
-        <v>189</v>
-      </c>
-      <c r="V1" t="s">
-        <v>190</v>
-      </c>
-      <c r="W1" t="s">
-        <v>191</v>
-      </c>
-      <c r="X1" t="s">
-        <v>192</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>193</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>194</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>195</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>196</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>197</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>198</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>199</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>200</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>201</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>202</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>203</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>204</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>205</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>206</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>207</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>208</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>209</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>210</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>211</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>212</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>213</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>214</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>215</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>216</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>217</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>218</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>219</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>220</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="2" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>998</v>
-      </c>
-      <c r="B2">
-        <v>17</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>20150101</v>
-      </c>
-      <c r="F2">
-        <v>99999999</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>6</v>
-      </c>
-      <c r="I2">
-        <v>82</v>
-      </c>
-      <c r="J2" t="s">
-        <v>222</v>
-      </c>
-      <c r="K2" t="s">
-        <v>223</v>
-      </c>
-      <c r="L2" t="s">
-        <v>224</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>1</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>999</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
-      <c r="AA2">
-        <v>0</v>
-      </c>
-      <c r="AB2">
-        <v>0</v>
-      </c>
-      <c r="AC2">
-        <v>1</v>
-      </c>
-      <c r="AD2">
-        <v>0</v>
-      </c>
-      <c r="AE2">
-        <v>3</v>
-      </c>
-      <c r="AF2">
-        <v>0</v>
-      </c>
-      <c r="AG2">
-        <v>0</v>
-      </c>
-      <c r="AH2">
-        <v>0</v>
-      </c>
-      <c r="AI2">
-        <v>0</v>
-      </c>
-      <c r="AJ2">
-        <v>0</v>
-      </c>
-      <c r="AK2">
-        <v>0</v>
-      </c>
-      <c r="AL2">
-        <v>0</v>
-      </c>
-      <c r="AM2">
-        <v>0</v>
-      </c>
-      <c r="AN2">
-        <v>0</v>
-      </c>
-      <c r="AO2">
-        <v>0</v>
-      </c>
-      <c r="AP2">
-        <v>1</v>
-      </c>
-      <c r="AQ2" s="1">
-        <v>42150</v>
-      </c>
-      <c r="AR2">
-        <v>99997</v>
-      </c>
-      <c r="AT2" s="1">
-        <v>42150</v>
-      </c>
-      <c r="AU2">
-        <v>99997</v>
-      </c>
-      <c r="AW2">
-        <v>11</v>
-      </c>
-      <c r="AX2">
-        <v>0</v>
-      </c>
-      <c r="AY2">
-        <v>0</v>
-      </c>
-      <c r="AZ2">
-        <v>1</v>
-      </c>
-      <c r="BA2">
-        <v>0</v>
-      </c>
-      <c r="BB2">
-        <v>0</v>
-      </c>
-      <c r="BC2">
-        <v>0</v>
-      </c>
-      <c r="BD2">
-        <v>0</v>
-      </c>
-      <c r="BE2">
-        <v>0</v>
-      </c>
-      <c r="BF2">
-        <v>0</v>
-      </c>
-      <c r="BG2">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>